<commit_message>
Updated Kasboek Diana '25, created Voorraad Repetitieruimte '25
</commit_message>
<xml_diff>
--- a/Files/Kasboek Diana '25.xlsx
+++ b/Files/Kasboek Diana '25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\DeMijnGang\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82EF155-CCC4-433C-92C5-02D8FAF4B160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61931287-5DE3-452A-A049-ED072458B680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1540,14 +1540,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="25">
-        <f>C4 - C5</f>
-        <v>1037.9100000000001</v>
+        <f>DEC!K35</f>
+        <v>3406.97</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="25">
-        <f>F4 + F5</f>
+        <f>DEC!H35</f>
         <v>0</v>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C8" s="14">
         <f>C6 + F6</f>
-        <v>1037.9100000000001</v>
+        <v>3406.97</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -9067,7 +9067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EDC514-F53A-4A12-B987-0F019A2BB10C}">
   <dimension ref="B2:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9942,7 +9944,7 @@
   <dimension ref="B2:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>